<commit_message>
3rd Version Please enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/FLOW CHART ASK UR Digram.xlsx
+++ b/FLOW CHART ASK UR Digram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38EEDC02-0352-44B2-BF22-2CB1A97DAC75}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AB6698-0638-40C6-B290-9DC06E473B82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" activeTab="3" xr2:uid="{A7327C89-5CCE-4692-B931-265BEBF5A6A3}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="84">
   <si>
     <t>Flow Digram</t>
   </si>
@@ -157,19 +157,130 @@
     <t xml:space="preserve">Cancel Appointment </t>
   </si>
   <si>
-    <t xml:space="preserve">Table - Patient </t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
     <t xml:space="preserve">int </t>
   </si>
   <si>
     <t>varchar</t>
   </si>
   <si>
-    <t>Enum</t>
+    <t>Patient Table</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country </t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Mob no.</t>
+  </si>
+  <si>
+    <t>Pid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Did </t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City </t>
+  </si>
+  <si>
+    <t xml:space="preserve">State </t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialisation </t>
+  </si>
+  <si>
+    <t>Fees</t>
+  </si>
+  <si>
+    <t>Langauges</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>(age(cal))</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>enum</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Registration Number</t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t>Doctor Time Table</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Slot Duration</t>
+  </si>
+  <si>
+    <t>Break Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holidays </t>
+  </si>
+  <si>
+    <t>14:00:00-15:00:00</t>
+  </si>
+  <si>
+    <t>Appoint Book</t>
+  </si>
+  <si>
+    <t>Did</t>
+  </si>
+  <si>
+    <t>Time Slot</t>
+  </si>
+  <si>
+    <t>Discription</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Medica Record and History</t>
+  </si>
+  <si>
+    <t>Admin Table</t>
+  </si>
+  <si>
+    <t>Aid</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -218,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,6 +375,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -447,6 +564,25 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3019,16 +3155,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>246016</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>202473</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>169817</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>367936</xdr:colOff>
+      <xdr:rowOff>115389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>324393</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>116477</xdr:rowOff>
+      <xdr:rowOff>62049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3043,7 +3179,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9999616" y="7016931"/>
+          <a:off x="10565673" y="6962503"/>
           <a:ext cx="1950720" cy="871946"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3814,9 +3950,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>2176</xdr:colOff>
+      <xdr:colOff>568233</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>169817</xdr:rowOff>
+      <xdr:rowOff>115389</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3835,7 +3971,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7713617" y="5866311"/>
-          <a:ext cx="3261359" cy="1150620"/>
+          <a:ext cx="3827416" cy="1096192"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4055,13 +4191,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
+      <xdr:colOff>51435</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:colOff>173355</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
@@ -4078,8 +4214,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="822960" y="3322320"/>
-          <a:ext cx="1950720" cy="840740"/>
+          <a:off x="661035" y="3288030"/>
+          <a:ext cx="1950720" cy="833120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4463,7 +4599,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:colOff>417195</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>109220</xdr:rowOff>
     </xdr:from>
@@ -4489,8 +4625,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1798320" y="2823845"/>
-          <a:ext cx="2217420" cy="464185"/>
+          <a:off x="1636395" y="2823845"/>
+          <a:ext cx="2379345" cy="464185"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5178,11 +5314,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DA79615-1009-4841-96BC-FF00CC43CD14}">
   <dimension ref="K29:L30"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T24" sqref="T24"/>
+    <sheetView topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="23" max="23" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="29" spans="11:12" x14ac:dyDescent="0.3">
       <c r="L29" s="1" t="s">
@@ -5209,7 +5349,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5221,19 +5361,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4EBDF6-474D-432D-9CA5-120821070B6D}">
-  <dimension ref="A1:AW28"/>
+  <dimension ref="A1:AW59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:H21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="8" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
     <col min="13" max="13" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.33203125" customWidth="1"/>
+    <col min="16" max="16" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.77734375" bestFit="1" customWidth="1"/>
@@ -5789,7 +5939,7 @@
     </row>
     <row r="18" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AK18" s="5"/>
       <c r="AL18" s="6"/>
@@ -5817,30 +5967,48 @@
       <c r="AP19" s="13"/>
     </row>
     <row r="20" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="A20" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" t="s">
+      <c r="D20" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I20" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J20" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="G20" t="s">
+      <c r="K20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H20" t="s">
+      <c r="L20" s="26" t="s">
         <v>14</v>
       </c>
+      <c r="M20" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
       <c r="AC20" s="5"/>
       <c r="AD20" s="6" t="s">
         <v>39</v>
@@ -5851,27 +6019,46 @@
       <c r="AH20" s="7"/>
     </row>
     <row r="21" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" t="s">
-        <v>27</v>
-      </c>
+      <c r="A21" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="6"/>
       <c r="AE21" s="6"/>
@@ -5880,6 +6067,22 @@
       <c r="AH21" s="7"/>
     </row>
     <row r="22" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A22" s="26"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="26"/>
+      <c r="K22" s="26"/>
+      <c r="L22" s="26"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
       <c r="AC22" s="5"/>
       <c r="AD22" s="2" t="s">
         <v>40</v>
@@ -5890,6 +6093,22 @@
       <c r="AH22" s="7"/>
     </row>
     <row r="23" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
       <c r="AE23" s="6"/>
@@ -5898,6 +6117,24 @@
       <c r="AH23" s="7"/>
     </row>
     <row r="24" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A24" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="26"/>
+      <c r="K24" s="26"/>
+      <c r="L24" s="26"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
       <c r="AE24" s="6"/>
@@ -5906,6 +6143,54 @@
       <c r="AH24" s="7"/>
     </row>
     <row r="25" spans="1:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="G25" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H25" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I25" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J25" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="K25" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="L25" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="M25" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="N25" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="O25" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="P25" s="26" t="s">
+        <v>66</v>
+      </c>
       <c r="AC25" s="5"/>
       <c r="AD25" s="11"/>
       <c r="AE25" s="18"/>
@@ -5914,6 +6199,54 @@
       <c r="AH25" s="7"/>
     </row>
     <row r="26" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A26" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="L26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="M26" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="O26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="P26" s="26" t="s">
+        <v>65</v>
+      </c>
       <c r="AC26" s="5"/>
       <c r="AD26" s="6"/>
       <c r="AE26" s="6"/>
@@ -5939,6 +6272,227 @@
       <c r="AG28" s="18"/>
       <c r="AH28" s="13"/>
     </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.3">
+      <c r="B32" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G32" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B33" s="26">
+        <v>1</v>
+      </c>
+      <c r="C33" s="30">
+        <v>44531</v>
+      </c>
+      <c r="D33" s="31">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E33" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="F33" s="26">
+        <v>30</v>
+      </c>
+      <c r="G33" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="26"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B34" s="26">
+        <v>1</v>
+      </c>
+      <c r="C34" s="30">
+        <v>44532</v>
+      </c>
+      <c r="D34" s="31">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E34" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="F34" s="26">
+        <v>30</v>
+      </c>
+      <c r="G34" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="29"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B35" s="26">
+        <v>1</v>
+      </c>
+      <c r="C35" s="30">
+        <v>44533</v>
+      </c>
+      <c r="D35" s="31">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E35" s="31">
+        <v>0.75</v>
+      </c>
+      <c r="F35" s="26">
+        <v>30</v>
+      </c>
+      <c r="G35" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H35" s="29"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B36" s="26"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B37" s="26"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="26"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5950,7 +6504,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="A3" sqref="A3:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Project start from here
</commit_message>
<xml_diff>
--- a/FLOW CHART ASK UR Digram.xlsx
+++ b/FLOW CHART ASK UR Digram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDBF5F11-7255-4454-89BC-CA8CE238F797}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7A0C05-2A86-4F08-8ABD-CFF46841A71B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" activeTab="3" xr2:uid="{A7327C89-5CCE-4692-B931-265BEBF5A6A3}"/>
   </bookViews>
@@ -5688,8 +5688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C4EBDF6-474D-432D-9CA5-120821070B6D}">
   <dimension ref="A1:AW135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:L26"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>